<commit_message>
Login full test cases Added
</commit_message>
<xml_diff>
--- a/Test_Case_Design/Login_Testing_Test_Cases.xlsx
+++ b/Test_Case_Design/Login_Testing_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wasana\University\Projects\QA-Portfolio\Test_Case_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CA1641-13E8-45D8-89C6-811F084471F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD62147B-9480-4F1C-8715-34A4430E72C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="164">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -297,13 +297,314 @@
   </si>
   <si>
     <t>Mandatory field appeared</t>
+  </si>
+  <si>
+    <t>TC-11</t>
+  </si>
+  <si>
+    <t>TS-14</t>
+  </si>
+  <si>
+    <t>Error message clarity</t>
+  </si>
+  <si>
+    <t>Verify that error messages are user-friendly, readable, and meaningful.</t>
+  </si>
+  <si>
+    <t>The error messages are user-friendly, readable, and meaningful.</t>
+  </si>
+  <si>
+    <t>1. Enter Email
+2. Enter Wrong Passsword
+3. Click Login</t>
+  </si>
+  <si>
+    <t>TC-12</t>
+  </si>
+  <si>
+    <t>Login button state</t>
+  </si>
+  <si>
+    <t>Verify that the Login button behavior is correct (enabled/disabled) based on input fields.</t>
+  </si>
+  <si>
+    <t>TS-15</t>
+  </si>
+  <si>
+    <t>Login button behavior is incorrect (enabled/disabled) based on input fields.</t>
+  </si>
+  <si>
+    <t>Login with minimum allowed password length</t>
+  </si>
+  <si>
+    <t>Login with maximum allowed password length</t>
+  </si>
+  <si>
+    <t>Login with special characters in password</t>
+  </si>
+  <si>
+    <t>Login with leading/trailing spaces</t>
+  </si>
+  <si>
+    <t>Multiple failed login attempts</t>
+  </si>
+  <si>
+    <t>Direct access without login</t>
+  </si>
+  <si>
+    <t>Logout functionality</t>
+  </si>
+  <si>
+    <t>Session expiration</t>
+  </si>
+  <si>
+    <t>Login on different browsers</t>
+  </si>
+  <si>
+    <t>Login on mobile devices</t>
+  </si>
+  <si>
+    <t>TC-13</t>
+  </si>
+  <si>
+    <t>TC-14</t>
+  </si>
+  <si>
+    <t>TC-15</t>
+  </si>
+  <si>
+    <t>TC-16</t>
+  </si>
+  <si>
+    <t>TC-17</t>
+  </si>
+  <si>
+    <t>TC-18</t>
+  </si>
+  <si>
+    <t>TC-19</t>
+  </si>
+  <si>
+    <t>TC-20</t>
+  </si>
+  <si>
+    <t>TC-21</t>
+  </si>
+  <si>
+    <t>TC-22</t>
+  </si>
+  <si>
+    <t>TS-16</t>
+  </si>
+  <si>
+    <t>TS-17</t>
+  </si>
+  <si>
+    <t>TS-18</t>
+  </si>
+  <si>
+    <t>TS-19</t>
+  </si>
+  <si>
+    <t>TS-20</t>
+  </si>
+  <si>
+    <t>TS-21</t>
+  </si>
+  <si>
+    <t>TS-22</t>
+  </si>
+  <si>
+    <t>TS-23</t>
+  </si>
+  <si>
+    <t>TS-24</t>
+  </si>
+  <si>
+    <t>TS-25</t>
+  </si>
+  <si>
+    <t>User is not logged in
+Application URL is accessible
+User knows a protected URL</t>
+  </si>
+  <si>
+    <t>Protected URL:</t>
+  </si>
+  <si>
+    <t>User should be redirected to the Login page
+Access to protected page should be denied</t>
+  </si>
+  <si>
+    <t>User is redirected to the Login page</t>
+  </si>
+  <si>
+    <t>User is logged in successfully
+User is on the Home page</t>
+  </si>
+  <si>
+    <t>1. Click on the Logout button
+2. Observe the application behavior
+3. Press browser back button</t>
+  </si>
+  <si>
+    <t>User should be logged out successfully
+User should be redirected to the Home page
+Back button should not allow access to previous one</t>
+  </si>
+  <si>
+    <t>User logged out and redirected to Login page</t>
+  </si>
+  <si>
+    <t>1. Open a web browser
+2. Enter the protected page URL directly in the address bar
+3. Press Enter</t>
+  </si>
+  <si>
+    <t>User is redirected to Home page after session expiration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is logged in
+Session timeout is configured </t>
+  </si>
+  <si>
+    <t>1. Login to the application
+2. Stay idle without any activity until session expires
+3. Try to access any protected page</t>
+  </si>
+  <si>
+    <t>Session should expire automatically
+User should be redirected to Login page
+Session expired message should be displayed</t>
+  </si>
+  <si>
+    <t>User is registered
+Browsers are installed</t>
+  </si>
+  <si>
+    <t>1. Open Chrome browser
+2. Login with valid credentials
+3. Repeat the same steps in Firefox and Edge</t>
+  </si>
+  <si>
+    <t>User should be able to login successfully on all browsers
+UI and functionality should be consistent</t>
+  </si>
+  <si>
+    <t>Login successful on all tested browsers</t>
+  </si>
+  <si>
+    <t>Browser types: Chrome, Firefox, Edge
+Email: wasu@gmail.com
+Password:wasana</t>
+  </si>
+  <si>
+    <t>User is registered
+Mobile device or emulator is available
+Internet connection is active</t>
+  </si>
+  <si>
+    <t>Login successful and UI displayed correctly on mobile</t>
+  </si>
+  <si>
+    <t>1. Open the application on a mobile browser
+2. Enter valid login credentials
+3. Tap the Login button</t>
+  </si>
+  <si>
+    <t>Device: Android / iOS
+Valid username and password</t>
+  </si>
+  <si>
+    <t>User should login successfully
+UI should be responsive and user-friendly</t>
+  </si>
+  <si>
+    <t>User is registered
+Minimum password length is defined 
+Login page is accessible</t>
+  </si>
+  <si>
+    <t>1. Open the login page
+2. Enter a valid email
+3. Enter a password with minimum allowed    length
+4. Click the Login button</t>
+  </si>
+  <si>
+    <t>User should login successfully
+User should be redirected to the Home Page</t>
+  </si>
+  <si>
+    <t>User logged in successfully with minimum password length</t>
+  </si>
+  <si>
+    <t>User is registered
+Maximum password length is defined (e.g., 20 characters)
+Login page is accessible</t>
+  </si>
+  <si>
+    <t>1. Open the login page
+2. Enter a valid email
+3 Enter a password with maximum allowed length
+4. Click the Login button</t>
+  </si>
+  <si>
+    <t>User should login successfully
+No validation error should be displayed</t>
+  </si>
+  <si>
+    <t>User logged in successfully with maximum password length</t>
+  </si>
+  <si>
+    <t>User logged in successfully using special characters in password</t>
+  </si>
+  <si>
+    <t>User is registered
+Password contains allowed special characters
+Login page is accessible</t>
+  </si>
+  <si>
+    <t>1. Open the login page
+2. Enter a valid email
+3. Enter a password containing special characters
+4. Click the Login button</t>
+  </si>
+  <si>
+    <t>User should login successfully
+System should accept special characters</t>
+  </si>
+  <si>
+    <t>User is registered
+Login page is accessible</t>
+  </si>
+  <si>
+    <t>1. Open the login page
+2. Enter valid email with leading/trailing spaces
+3. Enter valid password with leading/trailing spaces
+4. Click the Login button</t>
+  </si>
+  <si>
+    <t>System should trim spaces automatically
+User should login successfully OR show proper validation message</t>
+  </si>
+  <si>
+    <t>User account exists
+Maximum failed attempts limit is configured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: 
+Password: </t>
+  </si>
+  <si>
+    <t>System should display an error message
+Account should be temporarily locked OR CAPTCHA should appear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +628,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -390,6 +698,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,22 +991,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" customWidth="1"/>
     <col min="4" max="4" width="37.44140625" customWidth="1"/>
     <col min="5" max="5" width="36.88671875" customWidth="1"/>
     <col min="6" max="6" width="41.33203125" customWidth="1"/>
-    <col min="7" max="7" width="64.88671875" customWidth="1"/>
-    <col min="8" max="8" width="47.88671875" customWidth="1"/>
+    <col min="7" max="7" width="72.5546875" customWidth="1"/>
+    <col min="8" max="8" width="71.5546875" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1053,6 +1373,394 @@
       </c>
       <c r="K11" s="5"/>
     </row>
+    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>